<commit_message>
Added results for additional experiment
</commit_message>
<xml_diff>
--- a/docs/results/D2V_Validation_Embedding_Results.xlsx
+++ b/docs/results/D2V_Validation_Embedding_Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timcares/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{08B9E862-4926-134A-A336-599AD4F5C001}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44BC90E7-E1BC-184A-A10F-C1A99C6DE666}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="41280" yWindow="1760" windowWidth="28040" windowHeight="17440" xr2:uid="{67D46A3A-114F-5C4D-AEAD-D40E2A0D1361}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="37">
   <si>
     <t>Image</t>
   </si>
@@ -126,6 +126,27 @@
   </si>
   <si>
     <t xml:space="preserve">D2V validation test with KNN 20-Neighbors </t>
+  </si>
+  <si>
+    <t>Unpadded</t>
+  </si>
+  <si>
+    <t>0.8236</t>
+  </si>
+  <si>
+    <t>0.8962</t>
+  </si>
+  <si>
+    <t>0.8240</t>
+  </si>
+  <si>
+    <t>0.8972</t>
+  </si>
+  <si>
+    <t>0.1488</t>
+  </si>
+  <si>
+    <t>0.1484</t>
   </si>
 </sst>
 </file>
@@ -504,10 +525,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{680D38A3-923E-EA4B-9F9C-8EF5BFDD94C7}">
-  <dimension ref="A1:E55"/>
+  <dimension ref="A1:H55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -673,7 +694,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D33" t="s">
         <v>3</v>
       </c>
@@ -681,7 +702,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D34" t="s">
         <v>5</v>
       </c>
@@ -689,64 +710,94 @@
         <v>21</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C36" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F36" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D37" t="s">
         <v>3</v>
       </c>
       <c r="E37" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G37" t="s">
+        <v>3</v>
+      </c>
+      <c r="H37" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D38" t="s">
         <v>5</v>
       </c>
       <c r="E38" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G38" t="s">
+        <v>5</v>
+      </c>
+      <c r="H38" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C40" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F40" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D41" t="s">
         <v>3</v>
       </c>
       <c r="E41" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G41" t="s">
+        <v>3</v>
+      </c>
+      <c r="H41" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D42" t="s">
         <v>5</v>
       </c>
       <c r="E42" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G42" t="s">
+        <v>5</v>
+      </c>
+      <c r="H42" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C46" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D47" t="s">
         <v>3</v>
       </c>
@@ -754,30 +805,48 @@
         <v>26</v>
       </c>
     </row>
-    <row r="50" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C50" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="51" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="F50" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="51" spans="3:8" x14ac:dyDescent="0.2">
       <c r="D51" t="s">
         <v>3</v>
       </c>
       <c r="E51" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="54" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="G51" t="s">
+        <v>3</v>
+      </c>
+      <c r="H51" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="54" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C54" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="55" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="F54" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="55" spans="3:8" x14ac:dyDescent="0.2">
       <c r="D55" t="s">
         <v>3</v>
       </c>
       <c r="E55" t="s">
         <v>28</v>
+      </c>
+      <c r="G55" t="s">
+        <v>3</v>
+      </c>
+      <c r="H55" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>